<commit_message>
libelles colonnes en majuscule
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR_box.xlsx
+++ b/inst/template/BEUBOIS_CR_box.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="398" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="272" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,37 +27,37 @@
     <t>CLASSE</t>
   </si>
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Lots</t>
-  </si>
-  <si>
-    <t>Désignation</t>
-  </si>
-  <si>
-    <t>Représentant</t>
-  </si>
-  <si>
-    <t>Téléphone</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Courriel</t>
+    <t>NOM</t>
+  </si>
+  <si>
+    <t>LOT</t>
+  </si>
+  <si>
+    <t>DESIGNATION</t>
+  </si>
+  <si>
+    <t>REPRESENTANT</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
+  </si>
+  <si>
+    <t>FAX</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>Dif</t>
-  </si>
-  <si>
-    <t>Inv</t>
+    <t>DIF</t>
+  </si>
+  <si>
+    <t>INV</t>
   </si>
   <si>
     <t>C</t>
@@ -1487,8 +1487,8 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4021,7 +4021,7 @@
   </sheetPr>
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajouts au fichier excel et au readme - Etats : A valider, Validé, Annulé - DATEREALISATION
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR_box.xlsx
+++ b/inst/template/BEUBOIS_CR_box.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="272" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="346" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,13 +13,14 @@
     <sheet name="CEJOUR" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PLANS" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="PLANSNOTE" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PHOTOS" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="380">
   <si>
     <t>CLE</t>
   </si>
@@ -824,111 +825,141 @@
     <t>Epilobe</t>
   </si>
   <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>Etat</t>
+  </si>
+  <si>
+    <t>A faire</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>av</t>
+  </si>
+  <si>
+    <t>A valider</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Validé</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>Annulé</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Nouveau</t>
+  </si>
+  <si>
+    <t>ARCHI</t>
+  </si>
+  <si>
+    <t>Section Plans</t>
+  </si>
+  <si>
+    <t>01 PLANS ARCHITECTE</t>
+  </si>
+  <si>
+    <t>BETON</t>
+  </si>
+  <si>
+    <t>02 PLANS BETON</t>
+  </si>
+  <si>
+    <t>FLUID</t>
+  </si>
+  <si>
+    <t>03 PLANS FLUIDES</t>
+  </si>
+  <si>
+    <t>ELEC</t>
+  </si>
+  <si>
+    <t>04 PLANS ELEC</t>
+  </si>
+  <si>
+    <t>ENTREP</t>
+  </si>
+  <si>
+    <t>05 PLANS ENTREPRISES</t>
+  </si>
+  <si>
+    <t>PROTO</t>
+  </si>
+  <si>
+    <t>Soussection plans</t>
+  </si>
+  <si>
+    <t>00 PROTOTYPE</t>
+  </si>
+  <si>
+    <t>PLANS</t>
+  </si>
+  <si>
+    <t>01 PLANS</t>
+  </si>
+  <si>
+    <t>COUPES</t>
+  </si>
+  <si>
+    <t>02 COUPES</t>
+  </si>
+  <si>
+    <t>DETAILS</t>
+  </si>
+  <si>
+    <t>03 DETAILS</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>ECHEANCE</t>
+  </si>
+  <si>
+    <t>DATEREALISATION</t>
+  </si>
+  <si>
+    <t>PRIORITE</t>
+  </si>
+  <si>
+    <t>ETAT</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>ACTEUR</t>
+  </si>
+  <si>
+    <t>TACHE</t>
+  </si>
+  <si>
+    <t>Les blabla blabla</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
-    <t>Etat</t>
-  </si>
-  <si>
-    <t>A faire</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>Fait</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>ARCHI</t>
-  </si>
-  <si>
-    <t>Section Plans</t>
-  </si>
-  <si>
-    <t>01 PLANS ARCHITECTE</t>
-  </si>
-  <si>
-    <t>BETON</t>
-  </si>
-  <si>
-    <t>02 PLANS BETON</t>
-  </si>
-  <si>
-    <t>FLUID</t>
-  </si>
-  <si>
-    <t>03 PLANS FLUIDES</t>
-  </si>
-  <si>
-    <t>ELEC</t>
-  </si>
-  <si>
-    <t>04 PLANS ELEC</t>
-  </si>
-  <si>
-    <t>ENTREP</t>
-  </si>
-  <si>
-    <t>05 PLANS ENTREPRISES</t>
-  </si>
-  <si>
-    <t>PROTO</t>
-  </si>
-  <si>
-    <t>Soussection plans</t>
-  </si>
-  <si>
-    <t>00 PROTOTYPE</t>
-  </si>
-  <si>
-    <t>PLANS</t>
-  </si>
-  <si>
-    <t>01 PLANS</t>
-  </si>
-  <si>
-    <t>COUPES</t>
-  </si>
-  <si>
-    <t>02 COUPES</t>
-  </si>
-  <si>
-    <t>DETAILS</t>
-  </si>
-  <si>
-    <t>03 DETAILS</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>ECHEANCE</t>
-  </si>
-  <si>
-    <t>PRIORITE</t>
-  </si>
-  <si>
-    <t>ETAT</t>
-  </si>
-  <si>
-    <t>SECTION</t>
-  </si>
-  <si>
-    <t>ACTEUR</t>
-  </si>
-  <si>
-    <t>TACHE</t>
-  </si>
-  <si>
-    <t>Les blabla blabla</t>
-  </si>
-  <si>
     <t>ecp</t>
   </si>
   <si>
@@ -1140,6 +1171,12 @@
   </si>
   <si>
     <t>Pour déposer des fichiers aller dans le dossier « 0\_Dépôts » et remplir le formulaire. Un mail notifiant le dépôt d'un élément doit nous être transmis.</t>
+  </si>
+  <si>
+    <t>FICHIER</t>
+  </si>
+  <si>
+    <t>COMMENTAIRE</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1522,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="1" sqref="E1 C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2910,65 +2947,65 @@
       <c r="E46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="0"/>
-      <c r="C47" s="0"/>
+      <c r="A47" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="E47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
       <c r="E51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>279</v>
@@ -2976,58 +3013,106 @@
       <c r="E52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
-      <c r="B53" s="0"/>
-      <c r="C53" s="0"/>
+      <c r="A53" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="E53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>282</v>
+        <v>278</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="E54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>284</v>
+        <v>278</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="E55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>286</v>
+        <v>278</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="E56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C57" s="22" t="s">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="E57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E57" s="0"/>
+      <c r="B58" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="E58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="E59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="E60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="E61" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3066,181 +3151,192 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E1 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7125506072875"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1376518218624"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.331983805668"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>303</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="n">
         <v>42045</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="23"/>
+      <c r="E2" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="n">
         <v>42158</v>
       </c>
       <c r="B3" s="23" t="n">
         <v>42195</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>262</v>
-      </c>
+      <c r="C3" s="23"/>
       <c r="E3" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>297</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>307</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="n">
         <v>42092</v>
       </c>
       <c r="B4" s="23" t="n">
         <v>42108</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>299</v>
-      </c>
+      <c r="C4" s="23"/>
       <c r="D4" s="0" t="s">
-        <v>262</v>
+        <v>309</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="n">
         <v>42130</v>
       </c>
       <c r="B5" s="23" t="n">
         <v>42161</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>262</v>
-      </c>
+      <c r="C5" s="23"/>
       <c r="E5" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="n">
         <v>42136</v>
       </c>
       <c r="B6" s="23" t="n">
         <v>42167</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>262</v>
-      </c>
+      <c r="C6" s="23"/>
       <c r="E6" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>313</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="n">
         <v>42107</v>
       </c>
       <c r="B7" s="23" t="n">
         <v>42121</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="23"/>
+      <c r="E7" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="n">
         <v>42139</v>
       </c>
       <c r="B8" s="23" t="n">
         <v>42161</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>262</v>
-      </c>
+      <c r="C8" s="23"/>
       <c r="E8" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>306</v>
+      <c r="H8" s="0" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -3259,13 +3355,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2267206477733"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
@@ -3273,27 +3369,30 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>301</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="n">
         <v>42165</v>
       </c>
@@ -3306,11 +3405,12 @@
       <c r="D2" s="23" t="n">
         <v>42179</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="23"/>
+      <c r="G2" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="n">
         <v>42165</v>
       </c>
@@ -3321,14 +3421,15 @@
         <v>100</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="n">
         <v>42165</v>
       </c>
@@ -3341,50 +3442,53 @@
       <c r="D4" s="23" t="n">
         <v>42186</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="23"/>
+      <c r="G4" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D5" s="23" t="n">
         <v>42179</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="23"/>
+      <c r="G5" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D6" s="23" t="n">
         <v>42186</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="23"/>
+      <c r="G6" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>83</v>
@@ -3392,131 +3496,145 @@
       <c r="D7" s="23" t="n">
         <v>42199</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="23"/>
+      <c r="G7" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="D8" s="23" t="n">
         <v>42217</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="23"/>
+      <c r="G8" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="D9" s="23" t="n">
         <v>42179</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="23"/>
+      <c r="G9" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D10" s="23" t="n">
         <v>42228</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="23"/>
+      <c r="G10" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="D11" s="23" t="n">
         <v>42217</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="23"/>
+      <c r="G11" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D12" s="23"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D13" s="23"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D14" s="23"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D15" s="23"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D16" s="23"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D17" s="23"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D18" s="23"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D19" s="23"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="n">
         <v>42165</v>
       </c>
       <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3534,15 +3652,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="1" sqref="E1 C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.42105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4898785425101"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4331983805668"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9311740890688"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="24" width="10.5748987854251"/>
@@ -3551,39 +3669,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>289</v>
+        <v>297</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F2" s="25" t="n">
         <v>42114</v>
@@ -3591,17 +3712,17 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F3" s="25" t="n">
         <v>42128</v>
@@ -3609,17 +3730,17 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F4" s="25" t="n">
         <v>42128</v>
@@ -3627,17 +3748,17 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F5" s="25" t="n">
         <v>42128</v>
@@ -3645,17 +3766,17 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F6" s="25" t="n">
         <v>42128</v>
@@ -3663,17 +3784,17 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F7" s="25" t="n">
         <v>42128</v>
@@ -3681,17 +3802,17 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F8" s="25" t="n">
         <v>42128</v>
@@ -3699,17 +3820,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="F9" s="25" t="n">
         <v>42128</v>
@@ -3717,17 +3838,17 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="F10" s="25" t="n">
         <v>42128</v>
@@ -3735,17 +3856,17 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="F11" s="25" t="n">
         <v>42090</v>
@@ -3753,17 +3874,17 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="F12" s="27" t="n">
         <v>42142</v>
@@ -3771,17 +3892,17 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="F13" s="27" t="n">
         <v>42142</v>
@@ -3789,31 +3910,34 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F14" s="29" t="n">
         <v>42150</v>
       </c>
+      <c r="G14" s="0" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26" t="s">
@@ -3825,17 +3949,17 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="F16" s="27" t="n">
         <v>42121</v>
@@ -3843,31 +3967,34 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="F17" s="29" t="n">
         <v>42150</v>
       </c>
+      <c r="G17" s="0" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28" t="n">
@@ -3876,16 +4003,19 @@
       <c r="F18" s="29" t="n">
         <v>42150</v>
       </c>
+      <c r="G18" s="0" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28" t="n">
@@ -3894,16 +4024,19 @@
       <c r="F19" s="29" t="n">
         <v>42150</v>
       </c>
+      <c r="G19" s="0" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28" t="n">
@@ -3912,16 +4045,19 @@
       <c r="F20" s="29" t="n">
         <v>42150</v>
       </c>
+      <c r="G20" s="0" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="n">
@@ -3933,13 +4069,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="n">
@@ -3951,13 +4087,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="n">
@@ -3969,13 +4105,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="n">
@@ -3987,13 +4123,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="n">
@@ -4022,7 +4158,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="E1 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4033,12 +4169,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4046,22 +4182,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,7 +4205,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -4084,4 +4220,39 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="E1 D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- traitement nouveaux libelles : af, av, an - ajout date réalisation : Fait le xx/xx/xxx - fait non barré - traitement etat nouveau pour plans - ajout DATEREALISATION dans col_dates - ajout variable temp - ajout interlignes dans format_fun - ajout deplacement photos - retaillage dans dossier temp
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR_box.xlsx
+++ b/inst/template/BEUBOIS_CR_box.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="346" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="212" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,14 +13,13 @@
     <sheet name="CEJOUR" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PLANS" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="PLANSNOTE" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="PHOTOS" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="377">
   <si>
     <t>CLE</t>
   </si>
@@ -957,9 +956,6 @@
     <t>Les blabla blabla</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>ecp</t>
   </si>
   <si>
@@ -1171,12 +1167,6 @@
   </si>
   <si>
     <t>Pour déposer des fichiers aller dans le dossier « 0\_Dépôts » et remplir le formulaire. Un mail notifiant le dépôt d'un élément doit nous être transmis.</t>
-  </si>
-  <si>
-    <t>FICHIER</t>
-  </si>
-  <si>
-    <t>COMMENTAIRE</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1309,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1412,7 +1402,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1525,7 +1523,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="1" sqref="E1 C50"/>
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3154,14 +3152,14 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E1 C1"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7125506072875"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.331983805668"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="14.331983805668"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3172,7 +3170,7 @@
       <c r="B1" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="23" t="s">
         <v>299</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -3192,11 +3190,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="n">
+      <c r="A2" s="24" t="n">
         <v>42045</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
       <c r="E2" s="0" t="s">
         <v>267</v>
       </c>
@@ -3211,39 +3209,39 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="n">
+      <c r="A3" s="24" t="n">
         <v>42158</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="24" t="n">
         <v>42195</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="25"/>
       <c r="E3" s="0" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>258</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="H3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="n">
+        <v>42092</v>
+      </c>
+      <c r="B4" s="24" t="n">
+        <v>42108</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="0" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="n">
-        <v>42092</v>
-      </c>
-      <c r="B4" s="23" t="n">
-        <v>42108</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="0" t="s">
-        <v>309</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>258</v>
@@ -3252,19 +3250,19 @@
         <v>137</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="n">
+      <c r="A5" s="24" t="n">
         <v>42130</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="24" t="n">
         <v>42161</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="25"/>
       <c r="E5" s="0" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>260</v>
@@ -3273,38 +3271,40 @@
         <v>103</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
+        <v>42136</v>
+      </c>
+      <c r="B6" s="24" t="n">
+        <v>42167</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="E6" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="n">
-        <v>42136</v>
-      </c>
-      <c r="B6" s="23" t="n">
-        <v>42167</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="E6" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="n">
+      <c r="A7" s="24" t="n">
         <v>42107</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="24" t="n">
         <v>42121</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="24" t="n">
+        <v>42123</v>
+      </c>
       <c r="E7" s="0" t="s">
         <v>265</v>
       </c>
@@ -3315,19 +3315,19 @@
         <v>83</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="n">
+      <c r="A8" s="24" t="n">
         <v>42139</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="24" t="n">
         <v>42161</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="25"/>
       <c r="E8" s="0" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>256</v>
@@ -3336,7 +3336,7 @@
         <v>151</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3358,7 +3358,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3366,7 +3366,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2267206477733"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2267206477733"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,7 +3383,7 @@
       <c r="D1" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="23" t="s">
         <v>299</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -3393,7 +3394,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="n">
+      <c r="A2" s="24" t="n">
         <v>42165</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -3402,16 +3403,16 @@
       <c r="C2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="24" t="n">
         <v>42179</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="25"/>
       <c r="G2" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="n">
+      <c r="A3" s="24" t="n">
         <v>42165</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -3420,17 +3421,17 @@
       <c r="C3" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="0" t="s">
         <v>267</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="n">
+      <c r="A4" s="24" t="n">
         <v>42165</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -3439,202 +3440,202 @@
       <c r="C4" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="24" t="n">
         <v>42186</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="25"/>
       <c r="G4" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="n">
+        <v>42165</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="n">
+      <c r="D5" s="24" t="n">
+        <v>42179</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="G5" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>42179</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="G5" s="0" t="s">
+      <c r="B6" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="n">
+      <c r="D6" s="24" t="n">
+        <v>42186</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="G6" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>42186</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="G6" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="n">
-        <v>42165</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>324</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="23" t="n">
+      <c r="D7" s="24" t="n">
         <v>42199</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="25"/>
       <c r="G7" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>42165</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="n">
+      <c r="D8" s="24" t="n">
+        <v>42217</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="G8" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="D8" s="23" t="n">
+      <c r="B9" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="24" t="n">
+        <v>42179</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="G9" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="24" t="n">
+        <v>42165</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="24" t="n">
+        <v>42228</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="G10" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="24" t="n">
+        <v>42165</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="24" t="n">
         <v>42217</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="G8" s="0" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="n">
+      <c r="E11" s="25"/>
+      <c r="G11" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="D9" s="23" t="n">
-        <v>42179</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="G9" s="0" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="n">
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="D10" s="23" t="n">
-        <v>42228</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="G10" s="0" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="n">
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="D11" s="23" t="n">
-        <v>42217</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="G11" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="n">
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="n">
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="n">
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="n">
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="n">
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="n">
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="24" t="n">
         <v>42165</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="n">
-        <v>42165</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="n">
-        <v>42165</v>
-      </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="n">
-        <v>42165</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3655,7 +3656,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="1" sqref="E1 C30"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3663,7 +3664,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4898785425101"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4331983805668"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9311740890688"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="24" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="26" width="10.5748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
@@ -3672,18 +3673,18 @@
         <v>302</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="27" t="s">
         <v>297</v>
       </c>
       <c r="G1" s="0" t="s">
@@ -3695,18 +3696,18 @@
         <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="F2" s="25" t="n">
+      <c r="F2" s="27" t="n">
         <v>42114</v>
       </c>
     </row>
@@ -3715,16 +3716,16 @@
         <v>277</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="F3" s="25" t="n">
+        <v>339</v>
+      </c>
+      <c r="F3" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3733,16 +3734,16 @@
         <v>277</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="F4" s="25" t="n">
+        <v>339</v>
+      </c>
+      <c r="F4" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3751,16 +3752,16 @@
         <v>277</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="F5" s="25" t="n">
+        <v>339</v>
+      </c>
+      <c r="F5" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3769,16 +3770,16 @@
         <v>277</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="F6" s="25" t="n">
+        <v>339</v>
+      </c>
+      <c r="F6" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3787,16 +3788,16 @@
         <v>277</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="F7" s="25" t="n">
+        <v>345</v>
+      </c>
+      <c r="F7" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3805,16 +3806,16 @@
         <v>277</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="F8" s="25" t="n">
+        <v>345</v>
+      </c>
+      <c r="F8" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3823,16 +3824,16 @@
         <v>277</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="F9" s="25" t="n">
+        <v>348</v>
+      </c>
+      <c r="F9" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3841,16 +3842,16 @@
         <v>277</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="F10" s="25" t="n">
+        <v>348</v>
+      </c>
+      <c r="F10" s="27" t="n">
         <v>42128</v>
       </c>
     </row>
@@ -3859,16 +3860,16 @@
         <v>277</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="F11" s="25" t="n">
+        <v>351</v>
+      </c>
+      <c r="F11" s="27" t="n">
         <v>42090</v>
       </c>
     </row>
@@ -3877,16 +3878,16 @@
         <v>277</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C12" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
         <v>353</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26" t="s">
-        <v>354</v>
-      </c>
-      <c r="F12" s="27" t="n">
+      <c r="F12" s="29" t="n">
         <v>42142</v>
       </c>
     </row>
@@ -3895,16 +3896,16 @@
         <v>277</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>354</v>
       </c>
-      <c r="F13" s="27" t="n">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F13" s="29" t="n">
         <v>42142</v>
       </c>
     </row>
@@ -3913,16 +3914,16 @@
         <v>277</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C14" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
         <v>356</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28" t="s">
-        <v>357</v>
-      </c>
-      <c r="F14" s="29" t="n">
+      <c r="F14" s="31" t="n">
         <v>42150</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -3934,16 +3935,16 @@
         <v>277</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="27" t="n">
+      <c r="F15" s="29" t="n">
         <v>42137</v>
       </c>
     </row>
@@ -3952,16 +3953,16 @@
         <v>277</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>359</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>340</v>
-      </c>
-      <c r="F16" s="27" t="n">
+        <v>336</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="F16" s="29" t="n">
         <v>42121</v>
       </c>
     </row>
@@ -3970,16 +3971,16 @@
         <v>277</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28" t="s">
-        <v>352</v>
-      </c>
-      <c r="F17" s="29" t="n">
+        <v>336</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F17" s="31" t="n">
         <v>42150</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -3991,16 +3992,16 @@
         <v>277</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>361</v>
-      </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28" t="n">
+        <v>336</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>360</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="29" t="n">
+      <c r="F18" s="31" t="n">
         <v>42150</v>
       </c>
       <c r="G18" s="0" t="s">
@@ -4012,16 +4013,16 @@
         <v>277</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28" t="n">
+        <v>336</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="29" t="n">
+      <c r="F19" s="31" t="n">
         <v>42150</v>
       </c>
       <c r="G19" s="0" t="s">
@@ -4033,16 +4034,16 @@
         <v>277</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>363</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28" t="n">
+        <v>336</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="29" t="n">
+      <c r="F20" s="31" t="n">
         <v>42150</v>
       </c>
       <c r="G20" s="0" t="s">
@@ -4054,16 +4055,16 @@
         <v>277</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="25" t="n">
+      <c r="F21" s="27" t="n">
         <v>42080</v>
       </c>
     </row>
@@ -4072,16 +4073,16 @@
         <v>277</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>365</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>366</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="25" t="n">
+      <c r="F22" s="27" t="n">
         <v>42080</v>
       </c>
     </row>
@@ -4090,16 +4091,16 @@
         <v>277</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="25" t="n">
+      <c r="F23" s="27" t="n">
         <v>42080</v>
       </c>
     </row>
@@ -4108,16 +4109,16 @@
         <v>277</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="25" t="n">
+      <c r="F24" s="27" t="n">
         <v>42032</v>
       </c>
     </row>
@@ -4126,16 +4127,16 @@
         <v>277</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>369</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>370</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F25" s="25" t="n">
+      <c r="F25" s="27" t="n">
         <v>42101</v>
       </c>
     </row>
@@ -4158,23 +4159,23 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="E1 A4"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="120.251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="120.251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4182,22 +4183,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="32" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,7 +4206,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4220,39 +4221,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="E1 D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>379</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>